<commit_message>
aggiornamento medie indicatori simulativi
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/libFormula SIT/02_Inst_Variable_fixed.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/libFormula SIT/02_Inst_Variable_fixed.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michele.dessi\Desktop\libFormula SIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\libFormula SIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="470">
   <si>
     <t>Variable</t>
   </si>
@@ -1446,6 +1446,15 @@
   </si>
   <si>
     <t>264 - NPAF_IS_M_DOC_DB_L3M</t>
+  </si>
+  <si>
+    <t>CR0_Q_DER</t>
+  </si>
+  <si>
+    <t>IND_59</t>
+  </si>
+  <si>
+    <t>59 - CR0_Q_DER</t>
   </si>
 </sst>
 </file>
@@ -2786,10 +2795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N125"/>
+  <dimension ref="A1:N126"/>
   <sheetViews>
-    <sheetView topLeftCell="C97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124:D125"/>
+    <sheetView topLeftCell="A112" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8281,6 +8290,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>11</v>
+      </c>
+      <c r="B126" t="s">
+        <v>467</v>
+      </c>
+      <c r="C126" t="s">
+        <v>467</v>
+      </c>
+      <c r="D126" t="s">
+        <v>467</v>
+      </c>
+      <c r="E126" t="s">
+        <v>468</v>
+      </c>
+      <c r="F126" t="s">
+        <v>469</v>
+      </c>
+      <c r="G126">
+        <v>101</v>
+      </c>
+      <c r="H126" t="b">
+        <v>0</v>
+      </c>
+      <c r="I126" t="b">
+        <v>0</v>
+      </c>
+      <c r="J126" t="s">
+        <v>103</v>
+      </c>
+      <c r="K126" t="b">
+        <v>0</v>
+      </c>
+      <c r="L126" t="b">
+        <v>0</v>
+      </c>
+      <c r="M126" t="b">
+        <v>0</v>
+      </c>
+      <c r="N126" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -8290,10 +8343,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124:B125"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10424,6 +10477,23 @@
         <v>462</v>
       </c>
       <c r="F125" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>11</v>
+      </c>
+      <c r="B126" t="s">
+        <v>467</v>
+      </c>
+      <c r="C126" t="s">
+        <v>467</v>
+      </c>
+      <c r="E126" t="s">
+        <v>467</v>
+      </c>
+      <c r="F126" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>